<commit_message>
- added requiredments.txt - update environment layouts
</commit_message>
<xml_diff>
--- a/experimentResults/preliminary_experiment_PLAIN_2.xlsx
+++ b/experimentResults/preliminary_experiment_PLAIN_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofnottm-my.sharepoint.com/personal/psxsc27_nottingham_ac_uk/Documents/DIA/cw/experimentResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="327" documentId="11_1B0FC304FE797971BC6102DC18518DFFA12CB312" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ADE63F7-47EC-2A4A-85B9-5A522A2879BE}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="11_1B0FC304FE797971BC6102DC18518DFFA12CB312" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBD7AEEE-5CC9-DA44-801F-D23C888A4E28}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,22 +18,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet3!$I$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet3!$I$2:$I$101</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet3!$J$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet3!$J$2:$J$101</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet3!$K$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet3!$K$2:$K$101</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet3!$L$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet3!$L$2:$L$101</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet3!$J$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet3!$J$2:$J$101</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet3!$K$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet3!$K$2:$K$101</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet3!$L$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet3!$L$2:$L$101</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet3!$I$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet3!$I$2:$I$101</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">Sheet2!$C$16:$F$16,Sheet2!$D$17:$F$17,Sheet2!$E$18:$F$18,Sheet2!$F$19,Sheet2!$B$15:$F$15</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
@@ -82,7 +66,7 @@
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -9245,7 +9229,7 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13622,7 +13606,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" ref="C25:F29" si="2">C8*C15</f>
+        <f t="shared" ref="C25:F28" si="2">C8*C15</f>
         <v>0</v>
       </c>
       <c r="D25" s="2">

</xml_diff>